<commit_message>
Update file permissions and enhance project configuration
- Changed file permissions for multiple images and tables to executable (755).
- Updated `pyproject.toml` to improve linting and formatting configurations:
  - Expanded rule selection for better code quality.
  - Configured import sorting and docstring conventions.
  - Added project metadata including name, version, and description.
</commit_message>
<xml_diff>
--- a/conclusions/tables/nse_hydro_cluster_table.xlsx
+++ b/conclusions/tables/nse_hydro_cluster_table.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,32 +473,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>293</t>
+          <t>171</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.68</t>
+          <t>0.76</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>40</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>19</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>189</t>
+          <t>131</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>64.5%</t>
+          <t>76.6%</t>
         </is>
       </c>
     </row>
@@ -510,7 +510,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>113</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -520,7 +520,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>21</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -530,12 +530,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>92</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>81.7%</t>
+          <t>81.4%</t>
         </is>
       </c>
     </row>
@@ -547,32 +547,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>139</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.82</t>
+          <t>0.83</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>128</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>88.8%</t>
+          <t>92.1%</t>
         </is>
       </c>
     </row>
@@ -584,32 +584,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>239</t>
+          <t>156</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.64</t>
+          <t>0.71</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>76</t>
+          <t>32</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>6</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>124</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>68.2%</t>
+          <t>79.5%</t>
         </is>
       </c>
     </row>
@@ -621,32 +621,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>26</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.85</t>
+          <t>0.76</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>24</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>92.3%</t>
         </is>
       </c>
     </row>
@@ -658,32 +658,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>60</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.74</t>
+          <t>0.81</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>52</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>75.0%</t>
+          <t>86.7%</t>
         </is>
       </c>
     </row>
@@ -695,32 +695,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>102</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.69</t>
+          <t>0.78</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>88</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>86.3%</t>
         </is>
       </c>
     </row>
@@ -732,32 +732,69 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>107</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.79</t>
+          <t>0.41</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>62</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>25</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>45</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>89.2%</t>
+          <t>42.1%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Кластер 9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>122</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.60</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>58.2%</t>
         </is>
       </c>
     </row>

</xml_diff>